<commit_message>
Refactorization finished after testing. Some old new and old bugs have been fixed.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/mapping_example_maddalena.xlsx
+++ b/backend_tests/z_input_files/mapping_example_maddalena.xlsx
@@ -3969,10 +3969,10 @@
     <t xml:space="preserve">#MuSIASEM_EC</t>
   </si>
   <si>
-    <t xml:space="preserve">#VALUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Time_period</t>
+    <t xml:space="preserve">#sum_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#TIME_PERIOD</t>
   </si>
   <si>
     <t xml:space="preserve">#ds2.MuSIASEM_G</t>
@@ -4391,8 +4391,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4468,8 +4468,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4481,7 +4481,7 @@
   </sheetPr>
   <dimension ref="A1:S172"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P5" activeCellId="0" sqref="P5"/>
     </sheetView>
   </sheetViews>
@@ -9246,8 +9246,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -9355,8 +9355,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -9368,8 +9368,8 @@
   </sheetPr>
   <dimension ref="A1:P415"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18619,8 +18619,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -18633,7 +18633,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18641,7 +18641,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18718,8 +18719,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"Interfaces" command supporting multiple interfaces with same InterfaceType * Processor (v1 command) improved to support dataset expansion with case insensitive dimension naming * Module "test_command_container_files_execution.py" -> Unittests supported
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/mapping_example_maddalena.xlsx
+++ b/backend_tests/z_input_files/mapping_example_maddalena.xlsx
@@ -3966,7 +3966,7 @@
     <t xml:space="preserve">Int_In_Flow</t>
   </si>
   <si>
-    <t xml:space="preserve">#MuSIASEM_EC</t>
+    <t xml:space="preserve">#MuSIASEM_ec</t>
   </si>
   <si>
     <t xml:space="preserve">#sum_value</t>
@@ -4110,12 +4110,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -4391,8 +4391,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4468,8 +4468,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -9246,8 +9246,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -9355,8 +9355,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -18619,8 +18619,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -18633,7 +18633,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18719,8 +18719,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>